<commit_message>
updated best practices guide
</commit_message>
<xml_diff>
--- a/dmel_assembly_compare.xlsx
+++ b/dmel_assembly_compare.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniellekhost/github/intro_to_longread_seq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{53510269-8D42-3B4C-96C4-F5327FCD8F71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821CDCD1-120B-264F-B6A6-A68C656959E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="2720" windowWidth="28040" windowHeight="17440" activeTab="1"/>
+    <workbookView xWindow="1520" yWindow="1400" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dmel_assembly_compare" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="102">
   <si>
     <t>N50</t>
   </si>
@@ -266,9 +266,6 @@
     <t>~14 hrs</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>Assembly</t>
   </si>
   <si>
@@ -294,12 +291,48 @@
   </si>
   <si>
     <t>DNF</t>
+  </si>
+  <si>
+    <t>23 hrs</t>
+  </si>
+  <si>
+    <t>D. mel Flye</t>
+  </si>
+  <si>
+    <t>137.2Mb</t>
+  </si>
+  <si>
+    <t>24.3Mb</t>
+  </si>
+  <si>
+    <t>3.5 hrs</t>
+  </si>
+  <si>
+    <t>D. mel Flye + medaka</t>
+  </si>
+  <si>
+    <t>D. mel Flye + medaka + Hypo</t>
+  </si>
+  <si>
+    <t>Nasonia flye</t>
+  </si>
+  <si>
+    <t>13.3 Mb!</t>
+  </si>
+  <si>
+    <t>282.6 Mb</t>
+  </si>
+  <si>
+    <t>24.4 Mb</t>
+  </si>
+  <si>
+    <t>9 hr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1136,11 +1169,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="A1:G18"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1491,17 +1524,56 @@
         <v>80</v>
       </c>
     </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20">
+        <v>798</v>
+      </c>
+      <c r="E20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.73</v>
+      </c>
+      <c r="G20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.98599999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1514,7 +1586,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1620,11 +1692,11 @@
       <c r="E5" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>81</v>
+      <c r="F5" s="1">
+        <v>0.86</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1632,35 +1704,61 @@
         <v>70</v>
       </c>
       <c r="G6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" t="s">
         <v>85</v>
-      </c>
-      <c r="C7" t="s">
-        <v>86</v>
       </c>
       <c r="D7">
         <v>1716</v>
       </c>
       <c r="E7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F7" s="1">
         <v>0.26400000000000001</v>
       </c>
       <c r="G7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="G8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10">
+        <v>98</v>
+      </c>
+      <c r="E10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G10" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>